<commit_message>
Netzplan Übung 2 Lösungen
</commit_message>
<xml_diff>
--- a/Übungen/Netzplan_Übung2.xlsx
+++ b/Übungen/Netzplan_Übung2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Übung 1" sheetId="1" state="visible" r:id="rId3"/>
@@ -2161,8 +2161,8 @@
   </sheetPr>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2396,7 +2396,10 @@
         <f aca="false">C13-C10</f>
         <v>0</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="21" t="n">
+        <f aca="false">F10-C10</f>
+        <v>0</v>
+      </c>
       <c r="D12" s="18"/>
       <c r="E12" s="0"/>
       <c r="F12" s="19" t="n">
@@ -2407,7 +2410,10 @@
         <f aca="false">H13-H10</f>
         <v>0</v>
       </c>
-      <c r="H12" s="21"/>
+      <c r="H12" s="21" t="n">
+        <f aca="false">K10-H10</f>
+        <v>0</v>
+      </c>
       <c r="I12" s="0"/>
       <c r="J12" s="18"/>
       <c r="K12" s="19" t="n">
@@ -2418,7 +2424,10 @@
         <f aca="false">M13-M10</f>
         <v>0</v>
       </c>
-      <c r="M12" s="21"/>
+      <c r="M12" s="21" t="n">
+        <f aca="false">P10-M10</f>
+        <v>0</v>
+      </c>
       <c r="N12" s="0"/>
       <c r="O12" s="0"/>
       <c r="P12" s="19" t="n">
@@ -2582,7 +2591,10 @@
         <f aca="false">H19-H16</f>
         <v>3</v>
       </c>
-      <c r="H18" s="21"/>
+      <c r="H18" s="21" t="n">
+        <f aca="false">K10-H16</f>
+        <v>3</v>
+      </c>
       <c r="I18" s="0"/>
       <c r="J18" s="0"/>
       <c r="K18" s="0"/>
@@ -2949,7 +2961,7 @@
   </sheetPr>
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>